<commit_message>
Docs: Refeito os resultados com as medidas mais precisas e com a correção da fórmula do fator de delaminação pela area
</commit_message>
<xml_diff>
--- a/results/fEntrada.xlsx
+++ b/results/fEntrada.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perob\Documents\programação\delamination_unesp\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perob\Documents\programação\GitHub\delamination_unesp\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502C54A0-F93F-4AB3-B55D-9900131B9F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B44EC3-025D-4F83-876D-3501BCEC239B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{3D016B7E-74DE-4B84-A1A1-2ED0A21F6D3B}"/>
   </bookViews>
@@ -502,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC316C3-6D67-4241-A675-3FD94F5829CC}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,13 +527,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>1.1182939999999999</v>
+        <v>1.1055999999999999</v>
       </c>
       <c r="C2" s="2">
-        <v>0.54359999999999997</v>
+        <v>0.1105</v>
       </c>
       <c r="D2" s="2">
-        <v>2.8730000000000002</v>
+        <v>3.1318000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -541,13 +541,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>1.0924</v>
+        <v>1.1035999999999999</v>
       </c>
       <c r="C3" s="2">
-        <v>0.436</v>
+        <v>8.2699999999999996E-2</v>
       </c>
       <c r="D3" s="2">
-        <v>2.3041</v>
+        <v>2.3456000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -555,13 +555,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>1.0822000000000001</v>
+        <v>1.1161000000000001</v>
       </c>
       <c r="C4" s="2">
-        <v>0.36780000000000002</v>
+        <v>7.2599999999999998E-2</v>
       </c>
       <c r="D4" s="2">
-        <v>1.7565999999999999</v>
+        <v>2.0570599999999999</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -569,13 +569,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>1.0788</v>
+        <v>1.0656000000000001</v>
       </c>
       <c r="C5" s="2">
-        <v>0.43340000000000001</v>
+        <v>8.2799999999999999E-2</v>
       </c>
       <c r="D5" s="2">
-        <v>1.9823</v>
+        <v>2.3462999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -583,13 +583,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>1.0738000000000001</v>
+        <v>1.0817000000000001</v>
       </c>
       <c r="C6" s="2">
-        <v>0.54190000000000005</v>
+        <v>9.4299999999999995E-2</v>
       </c>
       <c r="D6" s="3">
-        <v>2.3140000000000001</v>
+        <v>2.6732999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -597,13 +597,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>1.0805</v>
+        <v>1.0825</v>
       </c>
       <c r="C7" s="2">
-        <v>0.59399999999999997</v>
+        <v>9.1899999999999996E-2</v>
       </c>
       <c r="D7" s="3">
-        <v>2.7770000000000001</v>
+        <v>2.0644</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -611,13 +611,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>1.0789</v>
+        <v>1.0518000000000001</v>
       </c>
       <c r="C8" s="2">
-        <v>0.48370000000000002</v>
+        <v>6.3100000000000003E-2</v>
       </c>
       <c r="D8" s="3">
-        <v>2.2086999999999999</v>
+        <v>1.7904</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -625,13 +625,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>1.0806</v>
+        <v>1.0742</v>
       </c>
       <c r="C9" s="2">
-        <v>0.43608999999999998</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="D9" s="3">
-        <v>2.0352999999999999</v>
+        <v>1.9145000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -639,13 +639,13 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>1.0823</v>
+        <v>1.0688</v>
       </c>
       <c r="C10" s="2">
-        <v>0.42049999999999998</v>
+        <v>6.8699999999999997E-2</v>
       </c>
       <c r="D10" s="3">
-        <v>2.0051999999999999</v>
+        <v>1.9476</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -653,13 +653,13 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>1.0823</v>
+        <v>1.0835999999999999</v>
       </c>
       <c r="C11" s="2">
-        <v>0.44419999999999998</v>
+        <v>6.88E-2</v>
       </c>
       <c r="D11" s="3">
-        <v>2.1183000000000001</v>
+        <v>1.9505999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -667,13 +667,13 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>1.1057999999999999</v>
+        <v>1.0817000000000001</v>
       </c>
       <c r="C12" s="2">
-        <v>0.35630000000000001</v>
+        <v>7.7899999999999997E-2</v>
       </c>
       <c r="D12" s="3">
-        <v>2.2092000000000001</v>
+        <v>2.2097000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -681,13 +681,13 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>1.1057999999999999</v>
+        <v>1.09009</v>
       </c>
       <c r="C13" s="2">
-        <v>0.25559999999999999</v>
+        <v>6.4049999999999996E-2</v>
       </c>
       <c r="D13" s="3">
-        <v>1.5847</v>
+        <v>1.8147</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -695,13 +695,13 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>1.1092</v>
+        <v>1.0783</v>
       </c>
       <c r="C14" s="2">
-        <v>0.31440000000000001</v>
+        <v>8.1500000000000003E-2</v>
       </c>
       <c r="D14" s="3">
-        <v>2.0148000000000001</v>
+        <v>2.3113000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -709,13 +709,13 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>1.0755999999999999</v>
+        <v>1.0667</v>
       </c>
       <c r="C15" s="2">
-        <v>0.53790000000000004</v>
+        <v>8.3199999999999996E-2</v>
       </c>
       <c r="D15" s="3">
-        <v>2.3479999999999999</v>
+        <v>2.3580999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -723,13 +723,13 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>1.0806</v>
+        <v>1.0658000000000001</v>
       </c>
       <c r="C16" s="2">
-        <v>0.443</v>
+        <v>6.5799999999999997E-2</v>
       </c>
       <c r="D16" s="3">
-        <v>2.0674999999999999</v>
+        <v>1.8652</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -737,13 +737,13 @@
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>1.0823</v>
+        <v>1.0808</v>
       </c>
       <c r="C17" s="2">
-        <v>0.53569999999999995</v>
+        <v>7.9009999999999997E-2</v>
       </c>
       <c r="D17" s="3">
-        <v>2.5543999999999998</v>
+        <v>2.2385999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -751,13 +751,13 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>1.0974699999999999</v>
+        <v>1.1156999999999999</v>
       </c>
       <c r="C18" s="2">
-        <v>0.62029999999999996</v>
+        <v>0.1171</v>
       </c>
       <c r="D18" s="3">
-        <v>2.5264000000000002</v>
+        <v>3.3200099999999999</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -765,13 +765,13 @@
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>1.0941000000000001</v>
+        <v>1.0665</v>
       </c>
       <c r="C19" s="2">
-        <v>0.34939999999999999</v>
+        <v>7.0800000000000002E-2</v>
       </c>
       <c r="D19" s="3">
-        <v>1.915</v>
+        <v>2.0082</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -779,13 +779,13 @@
         <v>20</v>
       </c>
       <c r="B20" s="2">
-        <v>1.0872999999999999</v>
+        <v>1.0650999999999999</v>
       </c>
       <c r="C20" s="2">
-        <v>0.38040000000000002</v>
+        <v>7.0599999999999996E-2</v>
       </c>
       <c r="D20" s="3">
-        <v>1.9296</v>
+        <v>2.0028000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -793,13 +793,13 @@
         <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>1.0872999999999999</v>
+        <v>1.0889</v>
       </c>
       <c r="C21" s="2">
-        <v>0.48708000000000001</v>
+        <v>0.1053</v>
       </c>
       <c r="D21" s="3">
-        <v>2.4706999999999999</v>
+        <v>2.9847000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -807,13 +807,13 @@
         <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>1.0956999999999999</v>
+        <v>1.1477999999999999</v>
       </c>
       <c r="C22" s="2">
-        <v>0.42502000000000001</v>
+        <v>0.1003</v>
       </c>
       <c r="D22" s="3">
-        <v>2.3725999999999998</v>
+        <v>2.8430599999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>